<commit_message>
cap nhat commit lan2
</commit_message>
<xml_diff>
--- a/Tien Trinh.xlsx
+++ b/Tien Trinh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macos/Desktop/Report/Baocao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macos/Desktop/Report/BaocaoTieuLuan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6B207-97EF-2D48-B0FC-1EE40406690B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD17DB2B-FF9F-1544-AADF-0DBABF6CB4EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16100" xr2:uid="{B2DBE721-EF54-2D41-B34A-A99403E65C95}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Mo ta he thong: db, ngon ngu, </t>
+  </si>
+  <si>
+    <t>3. Giao dien</t>
+  </si>
+  <si>
+    <t>1. Hien trang: cac ung dung tuong tu</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33827E2-9824-0743-B508-F79F82222A08}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -488,6 +497,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:B4"/>

</xml_diff>